<commit_message>
Count RDS files diet and virus
</commit_message>
<xml_diff>
--- a/DEGCounts.xlsx
+++ b/DEGCounts.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrutter/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lrutter/Desktop/HoneyBeePaper/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="460" windowWidth="15780" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="9600" yWindow="460" windowWidth="15780" windowHeight="14480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="43">
   <si>
     <t>C higher</t>
   </si>
@@ -72,6 +72,90 @@
   </si>
   <si>
     <t>VR higher</t>
+  </si>
+  <si>
+    <t>GDV</t>
+  </si>
+  <si>
+    <t>GDC</t>
+  </si>
+  <si>
+    <t>GEV</t>
+  </si>
+  <si>
+    <t>GEC</t>
+  </si>
+  <si>
+    <t>GLV</t>
+  </si>
+  <si>
+    <t>GLC</t>
+  </si>
+  <si>
+    <t>RDC</t>
+  </si>
+  <si>
+    <t>RDR</t>
+  </si>
+  <si>
+    <t>RD_DIET</t>
+  </si>
+  <si>
+    <t>RE_DIET</t>
+  </si>
+  <si>
+    <t>RER</t>
+  </si>
+  <si>
+    <t>REC</t>
+  </si>
+  <si>
+    <t>RLC</t>
+  </si>
+  <si>
+    <t>RLR</t>
+  </si>
+  <si>
+    <t>RL_DIET</t>
+  </si>
+  <si>
+    <t>RDV</t>
+  </si>
+  <si>
+    <t>REV</t>
+  </si>
+  <si>
+    <t>RLV</t>
+  </si>
+  <si>
+    <t>RDN</t>
+  </si>
+  <si>
+    <t>REN</t>
+  </si>
+  <si>
+    <t>RLN</t>
+  </si>
+  <si>
+    <t>RD_VIRUS</t>
+  </si>
+  <si>
+    <t>RE_VIRUS</t>
+  </si>
+  <si>
+    <t>RL_VIRUS</t>
+  </si>
+  <si>
+    <t>GD_VIRUS</t>
+  </si>
+  <si>
+    <t>GE_VIRUS</t>
+  </si>
+  <si>
+    <t>GL_VIRUS</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -440,20 +524,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -464,7 +548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -477,8 +561,20 @@
       <c r="D3">
         <v>1914</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -492,8 +588,20 @@
         <f>B4+C4</f>
         <v>1721</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -507,8 +615,20 @@
         <f>B5+C5</f>
         <v>1640</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -519,7 +639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -532,8 +652,20 @@
       <c r="D8">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -546,8 +678,20 @@
       <c r="D9">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -560,8 +704,20 @@
       <c r="D10">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -575,7 +731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -588,8 +744,17 @@
       <c r="D13">
         <v>1019</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -603,8 +768,17 @@
         <f>SUM(B14:C14)</f>
         <v>730</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -617,6 +791,15 @@
       <c r="D15">
         <f>SUM(B15:C15)</f>
         <v>213</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Finsh 27 sets of DEG counts
</commit_message>
<xml_diff>
--- a/DEGCounts.xlsx
+++ b/DEGCounts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="460" windowWidth="15780" windowHeight="14480" tabRatio="500"/>
+    <workbookView xWindow="12760" yWindow="460" windowWidth="12620" windowHeight="14480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="43">
   <si>
     <t>C higher</t>
   </si>
@@ -526,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -753,6 +753,9 @@
       <c r="H13" t="s">
         <v>39</v>
       </c>
+      <c r="I13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -777,6 +780,9 @@
       <c r="H14" t="s">
         <v>40</v>
       </c>
+      <c r="I14" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -800,6 +806,9 @@
       </c>
       <c r="H15" t="s">
         <v>41</v>
+      </c>
+      <c r="I15" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>